<commit_message>
test: retrain model and modify some plot
</commit_message>
<xml_diff>
--- a/scatter_plot_data.xlsx
+++ b/scatter_plot_data.xlsx
@@ -399,10 +399,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>0.6889404444100309</v>
+        <v>0.6849394633827639</v>
       </c>
       <c r="B2">
-        <v>-0.1829455916235286</v>
+        <v>-0.1991029243373718</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -410,10 +410,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>0.5775022265471608</v>
+        <v>0.5650587182852636</v>
       </c>
       <c r="B3">
-        <v>-0.05839159723922704</v>
+        <v>-0.06584084882539695</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -421,10 +421,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>0.6309830845514436</v>
+        <v>0.6245551909211056</v>
       </c>
       <c r="B4">
-        <v>-0.1001562296519532</v>
+        <v>-0.08632136788447388</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -432,10 +432,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>-0.2510890274945253</v>
+        <v>-0.2345117572554915</v>
       </c>
       <c r="B5">
-        <v>-0.2389950098001536</v>
+        <v>-0.2665998187069245</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -443,10 +443,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>-0.2695169612851934</v>
+        <v>-0.2589725241732819</v>
       </c>
       <c r="B6">
-        <v>-0.1437333347236067</v>
+        <v>-0.1779256419194835</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -454,10 +454,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>-0.7129034657440501</v>
+        <v>-0.7201249446276253</v>
       </c>
       <c r="B7">
-        <v>0.4058776871201469</v>
+        <v>0.3772183004841598</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -465,10 +465,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>0.6535592592038475</v>
+        <v>0.6466334129013331</v>
       </c>
       <c r="B8">
-        <v>-0.1376496878158058</v>
+        <v>-0.134908415902441</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -476,10 +476,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>0.364754288056983</v>
+        <v>0.3606442897530804</v>
       </c>
       <c r="B9">
-        <v>-0.3082071694301536</v>
+        <v>-0.3188799451523878</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -487,10 +487,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>0.4166587630236908</v>
+        <v>0.410246938892516</v>
       </c>
       <c r="B10">
-        <v>0.2065006855391553</v>
+        <v>0.229056889345671</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -498,10 +498,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>0.2933605003466488</v>
+        <v>0.2862544619450913</v>
       </c>
       <c r="B11">
-        <v>-0.2477175706064525</v>
+        <v>-0.2284061395910275</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -509,10 +509,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>0.184120973600195</v>
+        <v>0.1808371859435602</v>
       </c>
       <c r="B12">
-        <v>-0.1923685382835642</v>
+        <v>-0.166652466706552</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -520,10 +520,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>0.2745210607732438</v>
+        <v>0.2697336635890121</v>
       </c>
       <c r="B13">
-        <v>0.08322080641018152</v>
+        <v>0.1154306147226161</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -531,10 +531,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>0.6790741372036004</v>
+        <v>0.670888990277257</v>
       </c>
       <c r="B14">
-        <v>0.1368948481777995</v>
+        <v>0.1787883884146712</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -542,10 +542,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>0.595371974530457</v>
+        <v>0.5854487155498511</v>
       </c>
       <c r="B15">
-        <v>0.08678145298443073</v>
+        <v>0.1125440473818617</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -553,10 +553,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>0.5656941643634787</v>
+        <v>0.5517370010855083</v>
       </c>
       <c r="B16">
-        <v>0.2717676312840759</v>
+        <v>0.3038217950457748</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -564,10 +564,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>-0.6580535003747043</v>
+        <v>-0.6240405139873535</v>
       </c>
       <c r="B17">
-        <v>-0.2779275686975652</v>
+        <v>-0.302052714101543</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -575,10 +575,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>-1.004754845739259</v>
+        <v>-0.9875921376171526</v>
       </c>
       <c r="B18">
-        <v>-0.1524044961022952</v>
+        <v>-0.1812925842203401</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -586,10 +586,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>-0.8873125628501063</v>
+        <v>-0.866190188123107</v>
       </c>
       <c r="B19">
-        <v>0.1085393594535942</v>
+        <v>0.09723211380751637</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -597,10 +597,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>-0.08995357804552147</v>
+        <v>-0.1332823399139532</v>
       </c>
       <c r="B20">
-        <v>0.5676365241209053</v>
+        <v>0.5118230380633275</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -608,10 +608,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>-0.02065729592402642</v>
+        <v>-0.06338179601277323</v>
       </c>
       <c r="B21">
-        <v>0.6508436333512563</v>
+        <v>0.6112955162195787</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -619,10 +619,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>-0.1415396958203645</v>
+        <v>-0.2005042146948365</v>
       </c>
       <c r="B22">
-        <v>0.7930759729502883</v>
+        <v>0.7323605047455362</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -630,10 +630,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>-0.3337115384159646</v>
+        <v>-0.336251093200891</v>
       </c>
       <c r="B23">
-        <v>0.002901944133357207</v>
+        <v>-0.02650226096424592</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -641,10 +641,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>-0.722685854572658</v>
+        <v>-0.7259298750208257</v>
       </c>
       <c r="B24">
-        <v>-0.01574522694998862</v>
+        <v>-0.05694830321198292</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -652,10 +652,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>-0.7000512227928392</v>
+        <v>-0.6929106210679973</v>
       </c>
       <c r="B25">
-        <v>0.03000923196213243</v>
+        <v>0.01234359705070682</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -663,10 +663,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>-0.04344648568651967</v>
+        <v>-0.04232784057148823</v>
       </c>
       <c r="B26">
-        <v>0.3619187220960364</v>
+        <v>0.3823063921776238</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -674,10 +674,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>0.05039016975932447</v>
+        <v>0.04809760750937995</v>
       </c>
       <c r="B27">
-        <v>0.3247752574551378</v>
+        <v>0.3560363359025702</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -685,10 +685,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>-0.1026980581307723</v>
+        <v>-0.106245711029184</v>
       </c>
       <c r="B28">
-        <v>0.4008630955548705</v>
+        <v>0.3999344601274747</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -696,10 +696,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>0.7127485312758878</v>
+        <v>0.7209813185170854</v>
       </c>
       <c r="B29">
-        <v>-0.299940570820114</v>
+        <v>-0.2434615191937689</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -707,10 +707,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>0.6975794727572563</v>
+        <v>0.7174471126313243</v>
       </c>
       <c r="B30">
-        <v>-0.3609077205750625</v>
+        <v>-0.2933019043270977</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -718,10 +718,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>0.5726794704200817</v>
+        <v>0.5780203090749736</v>
       </c>
       <c r="B31">
-        <v>-0.002539840512060881</v>
+        <v>0.06566434322344011</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -729,10 +729,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>0.2675847401630254</v>
+        <v>0.2960044013949111</v>
       </c>
       <c r="B32">
-        <v>-0.6999141324820751</v>
+        <v>-0.6980951988826228</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -740,10 +740,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>0.4662788406814203</v>
+        <v>0.512690011381488</v>
       </c>
       <c r="B33">
-        <v>-0.5683067775149607</v>
+        <v>-0.5494976633865244</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -751,10 +751,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>0.2924618730142013</v>
+        <v>0.2891464869000891</v>
       </c>
       <c r="B34">
-        <v>0.1468677891725502</v>
+        <v>0.1714496016819628</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -762,10 +762,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>-0.01895833347825198</v>
+        <v>-0.0448261808912408</v>
       </c>
       <c r="B35">
-        <v>0.8084167188976973</v>
+        <v>0.8290026607023141</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -773,10 +773,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>0.1140613281965582</v>
+        <v>0.08502485275273208</v>
       </c>
       <c r="B36">
-        <v>0.7261211437574716</v>
+        <v>0.7335503115396761</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -784,10 +784,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>-0.02905073153639848</v>
+        <v>-0.06117039983197099</v>
       </c>
       <c r="B37">
-        <v>1.109620900472308</v>
+        <v>1.116659517991056</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -795,10 +795,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>0.2942900677119638</v>
+        <v>0.3091181930606106</v>
       </c>
       <c r="B38">
-        <v>-0.3588981615925316</v>
+        <v>-0.3376110526412668</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -806,10 +806,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>0.04815873401729013</v>
+        <v>0.05254254876721959</v>
       </c>
       <c r="B39">
-        <v>-0.4303741470674043</v>
+        <v>-0.4249648084560749</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -817,10 +817,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>0.02697809437522838</v>
+        <v>0.02673934517832282</v>
       </c>
       <c r="B40">
-        <v>0.055601477467092</v>
+        <v>0.07166579357133096</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -828,10 +828,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>-1.550388735567559</v>
+        <v>-1.539254456937815</v>
       </c>
       <c r="B41">
-        <v>-0.2734320370438256</v>
+        <v>-0.3526991206138202</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -839,10 +839,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>-1.072787336626762</v>
+        <v>-1.033475458794422</v>
       </c>
       <c r="B42">
-        <v>-0.2436447988660605</v>
+        <v>-0.2763944990215589</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -850,10 +850,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>-1.288081253346697</v>
+        <v>-1.278190789698606</v>
       </c>
       <c r="B43">
-        <v>0.1881831081354073</v>
+        <v>0.175124116574576</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -861,10 +861,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>0.01156033610918556</v>
+        <v>0.0195678562708264</v>
       </c>
       <c r="B44">
-        <v>-0.1914719417321628</v>
+        <v>-0.2245625299727138</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -872,10 +872,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>0.01050004619518049</v>
+        <v>0.01318282603378855</v>
       </c>
       <c r="B45">
-        <v>-0.2284421108664247</v>
+        <v>-0.2837546252344044</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -883,10 +883,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>0.06140987619975832</v>
+        <v>0.0618279140029669</v>
       </c>
       <c r="B46">
-        <v>-0.009843012414753036</v>
+        <v>-0.02445490083995593</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -894,10 +894,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>-0.4981233808201197</v>
+        <v>-0.5119980098871939</v>
       </c>
       <c r="B47">
-        <v>0.2983078811740828</v>
+        <v>0.2661682160254962</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -905,10 +905,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>-0.6027806992417792</v>
+        <v>-0.6352772083663795</v>
       </c>
       <c r="B48">
-        <v>0.4782805221304743</v>
+        <v>0.453404078596716</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -916,10 +916,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>-0.4439470757313065</v>
+        <v>-0.4722461100116873</v>
       </c>
       <c r="B49">
-        <v>0.3230375999171629</v>
+        <v>0.279122002581923</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -927,10 +927,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>-0.01172908876828463</v>
+        <v>-0.3266625549695667</v>
       </c>
       <c r="B50">
-        <v>0.07438064078923282</v>
+        <v>-0.1501092302766737</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -938,10 +938,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>0.07162652016489157</v>
+        <v>-0.1560408068698211</v>
       </c>
       <c r="B51">
-        <v>0.0692620523624846</v>
+        <v>0.2708007831602191</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -949,10 +949,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>0.04525124753377139</v>
+        <v>-0.1756018799480444</v>
       </c>
       <c r="B52">
-        <v>0.04131462204359392</v>
+        <v>0.1099224377168769</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -960,10 +960,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>-0.4475267262161223</v>
+        <v>-0.4584236664313774</v>
       </c>
       <c r="B53">
-        <v>0.1487655924813596</v>
+        <v>0.1092754828058694</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -971,10 +971,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>-0.2511937164625611</v>
+        <v>-0.2534423222357183</v>
       </c>
       <c r="B54">
-        <v>0.09715299017822167</v>
+        <v>0.06235452610474378</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -982,10 +982,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>-0.533303216639006</v>
+        <v>-0.5454141002637584</v>
       </c>
       <c r="B55">
-        <v>0.4391753462174132</v>
+        <v>0.4427541957112568</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -993,10 +993,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>-0.6528065847625499</v>
+        <v>-0.6547746856944328</v>
       </c>
       <c r="B56">
-        <v>-0.01919523448672267</v>
+        <v>-0.09434073014922473</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1004,10 +1004,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>-0.5886094109089116</v>
+        <v>-0.5945984928895528</v>
       </c>
       <c r="B57">
-        <v>0.1237168866152482</v>
+        <v>0.06811016287993275</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1015,10 +1015,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>-0.815698080965198</v>
+        <v>-0.8531239763392103</v>
       </c>
       <c r="B58">
-        <v>0.5614068801533832</v>
+        <v>0.4951286519909539</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1026,10 +1026,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>0.1045046659967944</v>
+        <v>0.09872030016109988</v>
       </c>
       <c r="B59">
-        <v>0.2847115326565347</v>
+        <v>0.3002871554598612</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1037,10 +1037,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>0.3446120347528853</v>
+        <v>0.3424796572105233</v>
       </c>
       <c r="B60">
-        <v>0.08049619312132683</v>
+        <v>0.1160505799067888</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1048,10 +1048,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>-0.0349130048916664</v>
+        <v>-0.05160659142342377</v>
       </c>
       <c r="B61">
-        <v>0.4652450298570379</v>
+        <v>0.4800106132991139</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1059,10 +1059,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>0.898434457823757</v>
+        <v>0.8801730919641776</v>
       </c>
       <c r="B62">
-        <v>0.0580532505194211</v>
+        <v>0.03609583981068049</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1070,10 +1070,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>0.792106504613489</v>
+        <v>0.7758086415970472</v>
       </c>
       <c r="B63">
-        <v>0.0589631898893137</v>
+        <v>0.07208799780468694</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1081,10 +1081,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>0.7720240531590156</v>
+        <v>0.7511144076372137</v>
       </c>
       <c r="B64">
-        <v>0.1669531634146411</v>
+        <v>0.1624501251230925</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1092,10 +1092,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
-        <v>1.135463572861148</v>
+        <v>1.135443379570934</v>
       </c>
       <c r="B65">
-        <v>-0.04755454579389825</v>
+        <v>-0.003522691101171341</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1103,10 +1103,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
-        <v>1.168195860707616</v>
+        <v>1.17026208173516</v>
       </c>
       <c r="B66">
-        <v>-0.01244160321476302</v>
+        <v>0.01929857898866151</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1114,10 +1114,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67">
-        <v>0.9583568299005286</v>
+        <v>0.9538739132301215</v>
       </c>
       <c r="B67">
-        <v>0.2443217160245315</v>
+        <v>0.29696168142657</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1125,10 +1125,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68">
-        <v>0.3814626902907027</v>
+        <v>0.3828857730620085</v>
       </c>
       <c r="B68">
-        <v>-0.3207855164528798</v>
+        <v>-0.2954030181424511</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1136,10 +1136,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69">
-        <v>0.3640120321961007</v>
+        <v>0.362126180941679</v>
       </c>
       <c r="B69">
-        <v>-0.3508070211939578</v>
+        <v>-0.3156897180618245</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1147,10 +1147,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
-        <v>0.1740723739037976</v>
+        <v>0.1645013142594524</v>
       </c>
       <c r="B70">
-        <v>-0.1455156622441754</v>
+        <v>-0.1216366730677188</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1158,10 +1158,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71">
-        <v>0.04118896160764744</v>
+        <v>0.05074111224038222</v>
       </c>
       <c r="B71">
-        <v>0.4138191360752453</v>
+        <v>0.3736556828679657</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -1169,10 +1169,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72">
-        <v>-0.1472030397581223</v>
+        <v>-0.1464702433666526</v>
       </c>
       <c r="B72">
-        <v>0.2014988878192287</v>
+        <v>0.1362521542917942</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -1180,10 +1180,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73">
-        <v>-0.1015872335247511</v>
+        <v>-0.1007376647257374</v>
       </c>
       <c r="B73">
-        <v>0.437748554339067</v>
+        <v>0.3855515627973073</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -1191,10 +1191,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74">
-        <v>0.6721518097259617</v>
+        <v>0.6496090021466765</v>
       </c>
       <c r="B74">
-        <v>0.2609648468470647</v>
+        <v>0.2438977358638474</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -1202,10 +1202,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75">
-        <v>0.905256648424771</v>
+        <v>0.881906685353618</v>
       </c>
       <c r="B75">
-        <v>0.5243263325913307</v>
+        <v>0.5509925325652254</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -1213,10 +1213,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76">
-        <v>0.9187979798778065</v>
+        <v>0.896416820749269</v>
       </c>
       <c r="B76">
-        <v>0.4129755871188973</v>
+        <v>0.4426229596474919</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -1224,10 +1224,10 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77">
-        <v>-0.05021787629659223</v>
+        <v>-0.06460783381016667</v>
       </c>
       <c r="B77">
-        <v>0.08625442456782734</v>
+        <v>0.04803429170405102</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -1235,10 +1235,10 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78">
-        <v>0.260967018429766</v>
+        <v>0.2499581961675801</v>
       </c>
       <c r="B78">
-        <v>0.02168852388767865</v>
+        <v>0.02670945055760772</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -1246,10 +1246,10 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79">
-        <v>-0.001102130192146442</v>
+        <v>-0.01116904703340199</v>
       </c>
       <c r="B79">
-        <v>0.2312875672542916</v>
+        <v>0.2252241470738349</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -1257,10 +1257,10 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
-        <v>0.08685071374808707</v>
+        <v>0.08583435980130509</v>
       </c>
       <c r="B80">
-        <v>-0.001952401308721362</v>
+        <v>-0.05258366054926691</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -1268,10 +1268,10 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>0.1275477152036504</v>
+        <v>0.1293204016103882</v>
       </c>
       <c r="B81">
-        <v>0.01015135848257192</v>
+        <v>-0.006175430180779322</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -1279,10 +1279,10 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>-0.03705016526634269</v>
+        <v>-0.05994988922660358</v>
       </c>
       <c r="B82">
-        <v>0.3445315535404546</v>
+        <v>0.2905463612222434</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -1290,10 +1290,10 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>0.1442529569908702</v>
+        <v>0.1180286375245629</v>
       </c>
       <c r="B83">
-        <v>0.2771833759050105</v>
+        <v>0.2827005562375826</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -1301,10 +1301,10 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>0.2447462468746187</v>
+        <v>0.2158816396877321</v>
       </c>
       <c r="B84">
-        <v>0.04862674206081115</v>
+        <v>0.04367757473032467</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -1312,10 +1312,10 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>0.2483362606580602</v>
+        <v>0.2136926220885885</v>
       </c>
       <c r="B85">
-        <v>0.3491148847230536</v>
+        <v>0.3572378788949241</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -1323,10 +1323,10 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86">
-        <v>0.3373457278714681</v>
+        <v>0.3548263391596985</v>
       </c>
       <c r="B86">
-        <v>-0.5034849643677453</v>
+        <v>-0.4911729526334269</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -1334,10 +1334,10 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87">
-        <v>0.2840572516206158</v>
+        <v>0.2951000761515962</v>
       </c>
       <c r="B87">
-        <v>-0.5244009467366323</v>
+        <v>-0.5263188751636175</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -1345,10 +1345,10 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
-        <v>0.199945173238451</v>
+        <v>0.2041954592674095</v>
       </c>
       <c r="B88">
-        <v>-0.2189702186845195</v>
+        <v>-0.192014158825965</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -1356,10 +1356,10 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89">
-        <v>-0.7951703935664495</v>
+        <v>-0.8111199759022808</v>
       </c>
       <c r="B89">
-        <v>0.3005632950594099</v>
+        <v>0.2440612260257316</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -1367,10 +1367,10 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90">
-        <v>-0.4669784030350438</v>
+        <v>-0.4927410330606728</v>
       </c>
       <c r="B90">
-        <v>0.01983798393386536</v>
+        <v>-0.04609530610000886</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -1378,10 +1378,10 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>-0.579917677626877</v>
+        <v>-0.611504614251119</v>
       </c>
       <c r="B91">
-        <v>0.6688291428932541</v>
+        <v>0.610010393283131</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -1389,10 +1389,10 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92">
-        <v>-0.3638744027156818</v>
+        <v>-0.3593742394999968</v>
       </c>
       <c r="B92">
-        <v>-0.2113831643028271</v>
+        <v>-0.2208913762140443</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -1400,10 +1400,10 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>-0.3580483923376643</v>
+        <v>-0.3711639128566756</v>
       </c>
       <c r="B93">
-        <v>-0.1537592670996052</v>
+        <v>-0.1698290401552744</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -1411,10 +1411,10 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
-        <v>-0.1912766293371556</v>
+        <v>-0.1848300746664908</v>
       </c>
       <c r="B94">
-        <v>-0.04253586465366133</v>
+        <v>-0.05214672155860557</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -1422,10 +1422,10 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95">
-        <v>-0.2864534025355207</v>
+        <v>-0.2701446445757179</v>
       </c>
       <c r="B95">
-        <v>-0.08759018793521094</v>
+        <v>-0.07862985098891188</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -1433,10 +1433,10 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96">
-        <v>-0.1630269306881341</v>
+        <v>-0.1502706176677735</v>
       </c>
       <c r="B96">
-        <v>-0.1174115465889761</v>
+        <v>-0.1004571117116597</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -1444,10 +1444,10 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97">
-        <v>-0.2103565479389426</v>
+        <v>-0.2002956818906377</v>
       </c>
       <c r="B97">
-        <v>0.09909538757133893</v>
+        <v>0.1280004367126152</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -1455,10 +1455,10 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98">
-        <v>0.6669964675690693</v>
+        <v>0.6521623252971831</v>
       </c>
       <c r="B98">
-        <v>0.05127029007600024</v>
+        <v>0.01580688885859961</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -1466,10 +1466,10 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99">
-        <v>0.6405619650559884</v>
+        <v>0.6216924811517589</v>
       </c>
       <c r="B99">
-        <v>0.04427770362456659</v>
+        <v>0.01336976095869444</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -1477,10 +1477,10 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100">
-        <v>0.4373161442645173</v>
+        <v>0.4122220335971336</v>
       </c>
       <c r="B100">
-        <v>0.5270019860169672</v>
+        <v>0.5152103093522173</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -1488,10 +1488,10 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101">
-        <v>-0.1976017057280904</v>
+        <v>-0.2305782723783268</v>
       </c>
       <c r="B101">
-        <v>0.246552730872384</v>
+        <v>0.2337069688285544</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -1499,10 +1499,10 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102">
-        <v>-0.1917112518104415</v>
+        <v>-0.209234516852795</v>
       </c>
       <c r="B102">
-        <v>0.09878811489800056</v>
+        <v>0.08493338904973639</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -1510,10 +1510,10 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103">
-        <v>-0.3991604910773164</v>
+        <v>-0.4364225485459761</v>
       </c>
       <c r="B103">
-        <v>0.4662623725162559</v>
+        <v>0.4489926709352628</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -1521,10 +1521,10 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104">
-        <v>1.04203839571786</v>
+        <v>1.036565128568453</v>
       </c>
       <c r="B104">
-        <v>0.08976887238762064</v>
+        <v>0.116990705702547</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -1532,10 +1532,10 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105">
-        <v>0.9144524556661603</v>
+        <v>0.9015148203699467</v>
       </c>
       <c r="B105">
-        <v>0.124780861665915</v>
+        <v>0.1295893382577407</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -1543,10 +1543,10 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106">
-        <v>0.8738074284705675</v>
+        <v>0.8560125316122004</v>
       </c>
       <c r="B106">
-        <v>0.3609723247480551</v>
+        <v>0.3883151472901958</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -1554,10 +1554,10 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107">
-        <v>0.998339767114641</v>
+        <v>1.015706022475836</v>
       </c>
       <c r="B107">
-        <v>-0.02672938975689522</v>
+        <v>0.008625926480982636</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -1565,10 +1565,10 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108">
-        <v>0.8250033352760419</v>
+        <v>0.8328856972792754</v>
       </c>
       <c r="B108">
-        <v>-0.1584556972514979</v>
+        <v>-0.1600943670152082</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -1576,10 +1576,10 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109">
-        <v>0.7675822208927413</v>
+        <v>0.7803946862868113</v>
       </c>
       <c r="B109">
-        <v>0.1713678403513967</v>
+        <v>0.2108394791818624</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -1587,10 +1587,10 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110">
-        <v>-0.2185429871935816</v>
+        <v>-0.1708596743915371</v>
       </c>
       <c r="B110">
-        <v>-0.9724270404747609</v>
+        <v>-0.9892367527262015</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -1598,10 +1598,10 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111">
-        <v>-0.1437277297112541</v>
+        <v>-0.09201698899989189</v>
       </c>
       <c r="B111">
-        <v>-0.909584757789366</v>
+        <v>-0.9012788895032079</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -1609,10 +1609,10 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112">
-        <v>-0.3343708285099122</v>
+        <v>-0.2897043342213437</v>
       </c>
       <c r="B112">
-        <v>-0.5737675555666746</v>
+        <v>-0.5503893068899318</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -1620,10 +1620,10 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113">
-        <v>0.1874637307219955</v>
+        <v>0.1781018523135876</v>
       </c>
       <c r="B113">
-        <v>-0.2202402544270971</v>
+        <v>-0.2433564789856389</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -1631,10 +1631,10 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114">
-        <v>0.4449328905723671</v>
+        <v>0.4386358704643499</v>
       </c>
       <c r="B114">
-        <v>-0.1980083906291364</v>
+        <v>-0.2205378709587363</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -1642,10 +1642,10 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115">
-        <v>0.3060830929875375</v>
+        <v>0.2934811580849028</v>
       </c>
       <c r="B115">
-        <v>-0.1771110713157329</v>
+        <v>-0.191319370200487</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -1653,10 +1653,10 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116">
-        <v>0.3716657720861243</v>
+        <v>0.3469424995925356</v>
       </c>
       <c r="B116">
-        <v>0.4498183383532864</v>
+        <v>0.4175613124786963</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -1664,10 +1664,10 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117">
-        <v>0.1777564741595343</v>
+        <v>0.1450138976351243</v>
       </c>
       <c r="B117">
-        <v>0.5480034462770741</v>
+        <v>0.4909128502483159</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -1675,10 +1675,10 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118">
-        <v>0.2096969265201275</v>
+        <v>0.178245501832191</v>
       </c>
       <c r="B118">
-        <v>0.7666926409743623</v>
+        <v>0.7394327555775286</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -1686,10 +1686,10 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119">
-        <v>-0.01052679544788208</v>
+        <v>-0.02245775966624209</v>
       </c>
       <c r="B119">
-        <v>0.01308392654725572</v>
+        <v>0.01071916467087345</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -1697,10 +1697,10 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120">
-        <v>0.2932704056539731</v>
+        <v>0.2920980398039759</v>
       </c>
       <c r="B120">
-        <v>0.1647931113027314</v>
+        <v>0.2196143475829442</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -1708,10 +1708,10 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121">
-        <v>0.2387976869029465</v>
+        <v>0.2094502097234484</v>
       </c>
       <c r="B121">
-        <v>0.1396771788770002</v>
+        <v>0.1434745223855976</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -1719,10 +1719,10 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122">
-        <v>-0.8819019907495856</v>
+        <v>-0.8932278482581307</v>
       </c>
       <c r="B122">
-        <v>1.00120502467958</v>
+        <v>0.9916933095060462</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -1730,10 +1730,10 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123">
-        <v>-0.9609938526513492</v>
+        <v>-0.97501881849414</v>
       </c>
       <c r="B123">
-        <v>1.065224281225528</v>
+        <v>1.054515860259287</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -1741,10 +1741,10 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124">
-        <v>-0.9147935095331446</v>
+        <v>-0.9582389337939788</v>
       </c>
       <c r="B124">
-        <v>1.303512059557833</v>
+        <v>1.281363300290423</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -1752,10 +1752,10 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125">
-        <v>-0.4959433769700151</v>
+        <v>-0.4818119132923295</v>
       </c>
       <c r="B125">
-        <v>-0.4789796028277179</v>
+        <v>-0.523126287352121</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -1763,10 +1763,10 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126">
-        <v>-0.4960934648930667</v>
+        <v>-0.4760635744465669</v>
       </c>
       <c r="B126">
-        <v>-0.6271248920178606</v>
+        <v>-0.6732101569011085</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -1774,10 +1774,10 @@
     </row>
     <row r="127" spans="1:3">
       <c r="A127">
-        <v>-0.5087715772603566</v>
+        <v>-0.5168656767539291</v>
       </c>
       <c r="B127">
-        <v>0.1126256417140209</v>
+        <v>0.09257909375889554</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -1785,10 +1785,10 @@
     </row>
     <row r="128" spans="1:3">
       <c r="A128">
-        <v>-0.6162510183111761</v>
+        <v>-0.6011659660155485</v>
       </c>
       <c r="B128">
-        <v>-0.4526308023712861</v>
+        <v>-0.4761097793386792</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -1796,10 +1796,10 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129">
-        <v>-0.4684290876074221</v>
+        <v>-0.4531298160322063</v>
       </c>
       <c r="B129">
-        <v>-0.5886586100228081</v>
+        <v>-0.6096095778664337</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -1807,10 +1807,10 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130">
-        <v>-0.4932945222807322</v>
+        <v>-0.4878288616961627</v>
       </c>
       <c r="B130">
-        <v>-0.2175054627496272</v>
+        <v>-0.2008818100252591</v>
       </c>
       <c r="C130">
         <v>1</v>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="131" spans="1:3">
       <c r="A131">
-        <v>-0.3254172154483314</v>
+        <v>-0.3181603834639751</v>
       </c>
       <c r="B131">
-        <v>-0.5578215069329719</v>
+        <v>-0.5705238229771075</v>
       </c>
       <c r="C131">
         <v>1</v>
@@ -1829,10 +1829,10 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132">
-        <v>-0.344234475132951</v>
+        <v>-0.3083526370577707</v>
       </c>
       <c r="B132">
-        <v>-0.6926686351407749</v>
+        <v>-0.6839489489146803</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -1840,10 +1840,10 @@
     </row>
     <row r="133" spans="1:3">
       <c r="A133">
-        <v>-0.523910719669931</v>
+        <v>-0.5171019760795907</v>
       </c>
       <c r="B133">
-        <v>-0.1570898202809406</v>
+        <v>-0.1376606491187545</v>
       </c>
       <c r="C133">
         <v>1</v>
@@ -1851,10 +1851,10 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134">
-        <v>0.2521127704278663</v>
+        <v>0.2517245631002534</v>
       </c>
       <c r="B134">
-        <v>0.3881931263090784</v>
+        <v>0.4259826270748003</v>
       </c>
       <c r="C134">
         <v>1</v>
@@ -1862,10 +1862,10 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135">
-        <v>0.3931722920975639</v>
+        <v>0.3857063048136074</v>
       </c>
       <c r="B135">
-        <v>0.4632521967415708</v>
+        <v>0.4990807944420846</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -1873,10 +1873,10 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136">
-        <v>0.6811544470842952</v>
+        <v>0.6772606451619427</v>
       </c>
       <c r="B136">
-        <v>0.6505251327051808</v>
+        <v>0.7216101338719136</v>
       </c>
       <c r="C136">
         <v>1</v>
@@ -1884,10 +1884,10 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137">
-        <v>-0.3025258253408744</v>
+        <v>-0.2966445517025186</v>
       </c>
       <c r="B137">
-        <v>-0.1304309818002743</v>
+        <v>-0.1456130276046098</v>
       </c>
       <c r="C137">
         <v>1</v>
@@ -1895,10 +1895,10 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138">
-        <v>-0.09306086010205311</v>
+        <v>-0.08176064864386713</v>
       </c>
       <c r="B138">
-        <v>-0.150478906679501</v>
+        <v>-0.1570472105904818</v>
       </c>
       <c r="C138">
         <v>1</v>
@@ -1906,10 +1906,10 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139">
-        <v>-0.4105772425682614</v>
+        <v>-0.4119015716429104</v>
       </c>
       <c r="B139">
-        <v>0.2587329231300318</v>
+        <v>0.2718042610734023</v>
       </c>
       <c r="C139">
         <v>1</v>
@@ -1917,10 +1917,10 @@
     </row>
     <row r="140" spans="1:3">
       <c r="A140">
-        <v>-0.4816598990738347</v>
+        <v>-0.4366746068900758</v>
       </c>
       <c r="B140">
-        <v>-0.6937345943267796</v>
+        <v>-0.6947405101274688</v>
       </c>
       <c r="C140">
         <v>1</v>
@@ -1928,10 +1928,10 @@
     </row>
     <row r="141" spans="1:3">
       <c r="A141">
-        <v>-0.3738847188218598</v>
+        <v>-0.3237739028069292</v>
       </c>
       <c r="B141">
-        <v>-0.6849330513914652</v>
+        <v>-0.6727454375038453</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -1939,10 +1939,10 @@
     </row>
     <row r="142" spans="1:3">
       <c r="A142">
-        <v>-0.6290584863875486</v>
+        <v>-0.5887807937623287</v>
       </c>
       <c r="B142">
-        <v>-0.3992861748627456</v>
+        <v>-0.3841689879844706</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -1950,10 +1950,10 @@
     </row>
     <row r="143" spans="1:3">
       <c r="A143">
-        <v>0.3432428365172958</v>
+        <v>0.3560180639553726</v>
       </c>
       <c r="B143">
-        <v>-0.1158378542144307</v>
+        <v>-0.1115943036120555</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -1961,10 +1961,10 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144">
-        <v>0.3185348517752247</v>
+        <v>0.3335538759163428</v>
       </c>
       <c r="B144">
-        <v>0.01351559088834249</v>
+        <v>0.05211460037206617</v>
       </c>
       <c r="C144">
         <v>1</v>
@@ -1972,10 +1972,10 @@
     </row>
     <row r="145" spans="1:3">
       <c r="A145">
-        <v>0.384046162354124</v>
+        <v>0.3861585544728107</v>
       </c>
       <c r="B145">
-        <v>0.171400508719643</v>
+        <v>0.2137098540571035</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -1983,10 +1983,10 @@
     </row>
     <row r="146" spans="1:3">
       <c r="A146">
-        <v>-0.09059118230587718</v>
+        <v>-0.0690420771109314</v>
       </c>
       <c r="B146">
-        <v>0.2856453067052319</v>
+        <v>0.2794995937273235</v>
       </c>
       <c r="C146">
         <v>1</v>
@@ -1994,10 +1994,10 @@
     </row>
     <row r="147" spans="1:3">
       <c r="A147">
-        <v>-0.1726972938273136</v>
+        <v>-0.1588059145789799</v>
       </c>
       <c r="B147">
-        <v>0.3224982548297196</v>
+        <v>0.3134452595531677</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -2005,10 +2005,10 @@
     </row>
     <row r="148" spans="1:3">
       <c r="A148">
-        <v>-0.2973422183675852</v>
+        <v>-0.2790029368177408</v>
       </c>
       <c r="B148">
-        <v>0.3603872413693179</v>
+        <v>0.3490095587862821</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -2016,10 +2016,10 @@
     </row>
     <row r="149" spans="1:3">
       <c r="A149">
-        <v>0.0378929673611837</v>
+        <v>0.04616826958903115</v>
       </c>
       <c r="B149">
-        <v>-0.340436417604528</v>
+        <v>-0.3544063345754693</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -2027,10 +2027,10 @@
     </row>
     <row r="150" spans="1:3">
       <c r="A150">
-        <v>0.04375659399542994</v>
+        <v>0.06009037920939226</v>
       </c>
       <c r="B150">
-        <v>-0.4187401128659164</v>
+        <v>-0.4114788861838403</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -2038,10 +2038,10 @@
     </row>
     <row r="151" spans="1:3">
       <c r="A151">
-        <v>-0.109113095213091</v>
+        <v>-0.1178754369824656</v>
       </c>
       <c r="B151">
-        <v>0.04888404881634006</v>
+        <v>0.03905294909110639</v>
       </c>
       <c r="C151">
         <v>1</v>
@@ -2049,10 +2049,10 @@
     </row>
     <row r="152" spans="1:3">
       <c r="A152">
-        <v>1.094759433022756</v>
+        <v>1.132873912164566</v>
       </c>
       <c r="B152">
-        <v>-0.07819696483338409</v>
+        <v>0.0003827804548362774</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -2060,10 +2060,10 @@
     </row>
     <row r="153" spans="1:3">
       <c r="A153">
-        <v>1.003597861475926</v>
+        <v>1.03796533926095</v>
       </c>
       <c r="B153">
-        <v>-0.1678297892953944</v>
+        <v>-0.09136573030082339</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -2071,10 +2071,10 @@
     </row>
     <row r="154" spans="1:3">
       <c r="A154">
-        <v>1.019406273344577</v>
+        <v>1.036459705094383</v>
       </c>
       <c r="B154">
-        <v>0.3313719224844794</v>
+        <v>0.4107529518364904</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -2082,10 +2082,10 @@
     </row>
     <row r="155" spans="1:3">
       <c r="A155">
-        <v>-0.296178721354907</v>
+        <v>-0.2680626717832487</v>
       </c>
       <c r="B155">
-        <v>-0.3585068385000705</v>
+        <v>-0.3667009801937922</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -2093,10 +2093,10 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156">
-        <v>-0.3938703518737458</v>
+        <v>-0.3751060847276017</v>
       </c>
       <c r="B156">
-        <v>-0.4102806844672882</v>
+        <v>-0.4437803496266438</v>
       </c>
       <c r="C156">
         <v>1</v>
@@ -2104,10 +2104,10 @@
     </row>
     <row r="157" spans="1:3">
       <c r="A157">
-        <v>-0.4682574688912887</v>
+        <v>-0.4549648867906446</v>
       </c>
       <c r="B157">
-        <v>-0.09568853884361324</v>
+        <v>-0.114098605279905</v>
       </c>
       <c r="C157">
         <v>1</v>
@@ -2115,10 +2115,10 @@
     </row>
     <row r="158" spans="1:3">
       <c r="A158">
-        <v>-0.1915879940581803</v>
+        <v>-0.489117493484563</v>
       </c>
       <c r="B158">
-        <v>-0.4708192750432966</v>
+        <v>-0.6346148234840432</v>
       </c>
       <c r="C158">
         <v>1</v>
@@ -2126,10 +2126,10 @@
     </row>
     <row r="159" spans="1:3">
       <c r="A159">
-        <v>-0.1590830127515608</v>
+        <v>-0.06439150215702424</v>
       </c>
       <c r="B159">
-        <v>-0.3171313361337275</v>
+        <v>-0.7065330799930647</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -2137,10 +2137,10 @@
     </row>
     <row r="160" spans="1:3">
       <c r="A160">
-        <v>-0.2197543742423513</v>
+        <v>-0.5409129929774792</v>
       </c>
       <c r="B160">
-        <v>-0.3084190460393989</v>
+        <v>-0.2039759339930829</v>
       </c>
       <c r="C160">
         <v>1</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="161" spans="1:3">
       <c r="A161">
-        <v>-0.1153946851861138</v>
+        <v>-0.08981905013242181</v>
       </c>
       <c r="B161">
-        <v>-0.5808036470375384</v>
+        <v>-0.5856360148113232</v>
       </c>
       <c r="C161">
         <v>1</v>
@@ -2159,10 +2159,10 @@
     </row>
     <row r="162" spans="1:3">
       <c r="A162">
-        <v>-0.01799955888267768</v>
+        <v>0.007569555649956611</v>
       </c>
       <c r="B162">
-        <v>-0.7179786152287222</v>
+        <v>-0.7247660448695061</v>
       </c>
       <c r="C162">
         <v>1</v>
@@ -2170,10 +2170,10 @@
     </row>
     <row r="163" spans="1:3">
       <c r="A163">
-        <v>-0.0465191086450014</v>
+        <v>-0.02912367286431566</v>
       </c>
       <c r="B163">
-        <v>-0.281444746707619</v>
+        <v>-0.2863648502956309</v>
       </c>
       <c r="C163">
         <v>1</v>
@@ -2181,10 +2181,10 @@
     </row>
     <row r="164" spans="1:3">
       <c r="A164">
-        <v>0.4681086918380066</v>
+        <v>0.5022284621081431</v>
       </c>
       <c r="B164">
-        <v>-0.7151732625140045</v>
+        <v>-0.7365323941317033</v>
       </c>
       <c r="C164">
         <v>1</v>
@@ -2192,10 +2192,10 @@
     </row>
     <row r="165" spans="1:3">
       <c r="A165">
-        <v>0.2804740527321164</v>
+        <v>0.3033328215080442</v>
       </c>
       <c r="B165">
-        <v>-0.7063501063123828</v>
+        <v>-0.735158540618904</v>
       </c>
       <c r="C165">
         <v>1</v>
@@ -2203,10 +2203,10 @@
     </row>
     <row r="166" spans="1:3">
       <c r="A166">
-        <v>0.3292118948341826</v>
+        <v>0.3516926104838352</v>
       </c>
       <c r="B166">
-        <v>-0.4129332444617294</v>
+        <v>-0.4145841687489272</v>
       </c>
       <c r="C166">
         <v>1</v>
@@ -2214,10 +2214,10 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167">
-        <v>-0.1520936166847966</v>
+        <v>-0.1115272316629084</v>
       </c>
       <c r="B167">
-        <v>-0.7444541765535522</v>
+        <v>-0.748927877088387</v>
       </c>
       <c r="C167">
         <v>1</v>
@@ -2225,10 +2225,10 @@
     </row>
     <row r="168" spans="1:3">
       <c r="A168">
-        <v>-0.3544717031849199</v>
+        <v>-0.3197782587329236</v>
       </c>
       <c r="B168">
-        <v>-0.5769356270195695</v>
+        <v>-0.5783792489265854</v>
       </c>
       <c r="C168">
         <v>1</v>
@@ -2236,10 +2236,10 @@
     </row>
     <row r="169" spans="1:3">
       <c r="A169">
-        <v>0.04259575212072866</v>
+        <v>0.08118161734484866</v>
       </c>
       <c r="B169">
-        <v>-0.6850836761138651</v>
+        <v>-0.6523631657452348</v>
       </c>
       <c r="C169">
         <v>1</v>
@@ -2247,10 +2247,10 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170">
-        <v>-0.3634828875593391</v>
+        <v>-0.358375477014465</v>
       </c>
       <c r="B170">
-        <v>-0.1886082619099488</v>
+        <v>-0.2049299812262066</v>
       </c>
       <c r="C170">
         <v>1</v>
@@ -2258,10 +2258,10 @@
     </row>
     <row r="171" spans="1:3">
       <c r="A171">
-        <v>-0.2666630338755224</v>
+        <v>-0.2641165122541578</v>
       </c>
       <c r="B171">
-        <v>-0.1724667972172798</v>
+        <v>-0.1700689895202602</v>
       </c>
       <c r="C171">
         <v>1</v>
@@ -2269,10 +2269,10 @@
     </row>
     <row r="172" spans="1:3">
       <c r="A172">
-        <v>-0.3106780383843104</v>
+        <v>-0.3047163458176896</v>
       </c>
       <c r="B172">
-        <v>-0.1094256346807443</v>
+        <v>-0.09908314970212768</v>
       </c>
       <c r="C172">
         <v>1</v>
@@ -2280,10 +2280,10 @@
     </row>
     <row r="173" spans="1:3">
       <c r="A173">
-        <v>-0.3596990623688039</v>
+        <v>-0.1101684839007475</v>
       </c>
       <c r="B173">
-        <v>-0.9820971013358688</v>
+        <v>-0.8630546368504507</v>
       </c>
       <c r="C173">
         <v>1</v>
@@ -2291,10 +2291,10 @@
     </row>
     <row r="174" spans="1:3">
       <c r="A174">
-        <v>-0.3731153452440873</v>
+        <v>-0.05838236083732567</v>
       </c>
       <c r="B174">
-        <v>-1.048665801626832</v>
+        <v>-0.9820903176506569</v>
       </c>
       <c r="C174">
         <v>1</v>
@@ -2302,10 +2302,10 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175">
-        <v>-0.2537398286392305</v>
+        <v>-0.1756151007235209</v>
       </c>
       <c r="B175">
-        <v>-0.7150631189671287</v>
+        <v>-0.5020560608887719</v>
       </c>
       <c r="C175">
         <v>1</v>
@@ -2313,10 +2313,10 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176">
-        <v>-0.4355539792226922</v>
+        <v>-0.4151286089960541</v>
       </c>
       <c r="B176">
-        <v>-0.3439998943671107</v>
+        <v>-0.3292891246652196</v>
       </c>
       <c r="C176">
         <v>1</v>
@@ -2324,10 +2324,10 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177">
-        <v>-0.4433548067159245</v>
+        <v>-0.4260105809583987</v>
       </c>
       <c r="B177">
-        <v>-0.3314119563361023</v>
+        <v>-0.3271840707964536</v>
       </c>
       <c r="C177">
         <v>1</v>
@@ -2335,10 +2335,10 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178">
-        <v>-0.4613537039417592</v>
+        <v>-0.4485427505169109</v>
       </c>
       <c r="B178">
-        <v>-0.05219400624460664</v>
+        <v>-0.02226650582778813</v>
       </c>
       <c r="C178">
         <v>1</v>
@@ -2346,10 +2346,10 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179">
-        <v>0.9983785686978947</v>
+        <v>0.9973673687089141</v>
       </c>
       <c r="B179">
-        <v>0.1221389211672208</v>
+        <v>0.1164799406383055</v>
       </c>
       <c r="C179">
         <v>1</v>
@@ -2357,10 +2357,10 @@
     </row>
     <row r="180" spans="1:3">
       <c r="A180">
-        <v>0.9634871016611422</v>
+        <v>0.9561847016666056</v>
       </c>
       <c r="B180">
-        <v>0.1654812840274126</v>
+        <v>0.1579923389270431</v>
       </c>
       <c r="C180">
         <v>1</v>
@@ -2368,10 +2368,10 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181">
-        <v>0.6837632890328629</v>
+        <v>0.6647968535288731</v>
       </c>
       <c r="B181">
-        <v>0.7046031093891942</v>
+        <v>0.705196329716874</v>
       </c>
       <c r="C181">
         <v>1</v>
@@ -2379,10 +2379,10 @@
     </row>
     <row r="182" spans="1:3">
       <c r="A182">
-        <v>0.698717739901755</v>
+        <v>0.7287546713751495</v>
       </c>
       <c r="B182">
-        <v>-0.5446063132553149</v>
+        <v>-0.5087708967895599</v>
       </c>
       <c r="C182">
         <v>1</v>
@@ -2390,10 +2390,10 @@
     </row>
     <row r="183" spans="1:3">
       <c r="A183">
-        <v>0.7005360091206727</v>
+        <v>0.7272385411933027</v>
       </c>
       <c r="B183">
-        <v>-0.5860135006983045</v>
+        <v>-0.5531728782949332</v>
       </c>
       <c r="C183">
         <v>1</v>
@@ -2401,10 +2401,10 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184">
-        <v>0.4936617067825517</v>
+        <v>0.524841302743456</v>
       </c>
       <c r="B184">
-        <v>-0.3131240342239922</v>
+        <v>-0.2835174917583682</v>
       </c>
       <c r="C184">
         <v>1</v>
@@ -2412,10 +2412,10 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185">
-        <v>-0.8527788087854912</v>
+        <v>-0.8908366237984007</v>
       </c>
       <c r="B185">
-        <v>1.142742887414892</v>
+        <v>1.154310209802062</v>
       </c>
       <c r="C185">
         <v>1</v>
@@ -2423,10 +2423,10 @@
     </row>
     <row r="186" spans="1:3">
       <c r="A186">
-        <v>-0.676446586717611</v>
+        <v>-0.7227072608711897</v>
       </c>
       <c r="B186">
-        <v>1.305076644486203</v>
+        <v>1.328608376718139</v>
       </c>
       <c r="C186">
         <v>1</v>
@@ -2434,10 +2434,10 @@
     </row>
     <row r="187" spans="1:3">
       <c r="A187">
-        <v>-0.7111182712914673</v>
+        <v>-0.7579157515216344</v>
       </c>
       <c r="B187">
-        <v>1.362664204527408</v>
+        <v>1.376444215325638</v>
       </c>
       <c r="C187">
         <v>1</v>
@@ -2445,10 +2445,10 @@
     </row>
     <row r="188" spans="1:3">
       <c r="A188">
-        <v>0.8753527678190784</v>
+        <v>0.8878752298515696</v>
       </c>
       <c r="B188">
-        <v>-0.2528368449049437</v>
+        <v>-0.1508364617535781</v>
       </c>
       <c r="C188">
         <v>1</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="189" spans="1:3">
       <c r="A189">
-        <v>0.9500918560833163</v>
+        <v>0.9712060494843722</v>
       </c>
       <c r="B189">
-        <v>-0.2422832154001674</v>
+        <v>-0.1505201564538232</v>
       </c>
       <c r="C189">
         <v>1</v>
@@ -2467,10 +2467,10 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190">
-        <v>0.8084830553990723</v>
+        <v>0.8177680840242236</v>
       </c>
       <c r="B190">
-        <v>0.2417758149408202</v>
+        <v>0.3664515731896665</v>
       </c>
       <c r="C190">
         <v>1</v>
@@ -2478,10 +2478,10 @@
     </row>
     <row r="191" spans="1:3">
       <c r="A191">
-        <v>-0.2731500567331556</v>
+        <v>-0.2839966763481408</v>
       </c>
       <c r="B191">
-        <v>0.6993773712559436</v>
+        <v>0.6590927542122472</v>
       </c>
       <c r="C191">
         <v>1</v>
@@ -2489,10 +2489,10 @@
     </row>
     <row r="192" spans="1:3">
       <c r="A192">
-        <v>-0.3612543687648696</v>
+        <v>-0.3737743494593119</v>
       </c>
       <c r="B192">
-        <v>0.6813858600538142</v>
+        <v>0.6402119188212992</v>
       </c>
       <c r="C192">
         <v>1</v>
@@ -2500,10 +2500,10 @@
     </row>
     <row r="193" spans="1:3">
       <c r="A193">
-        <v>-0.4912715678848145</v>
+        <v>-0.5282851723610879</v>
       </c>
       <c r="B193">
-        <v>0.8786596598128665</v>
+        <v>0.7947692511341758</v>
       </c>
       <c r="C193">
         <v>1</v>
@@ -2511,10 +2511,10 @@
     </row>
     <row r="194" spans="1:3">
       <c r="A194">
-        <v>-0.1163094908188673</v>
+        <v>-0.1466461634277894</v>
       </c>
       <c r="B194">
-        <v>0.420811246569898</v>
+        <v>0.3959585430674359</v>
       </c>
       <c r="C194">
         <v>1</v>
@@ -2522,10 +2522,10 @@
     </row>
     <row r="195" spans="1:3">
       <c r="A195">
-        <v>0.03277701294001312</v>
+        <v>0.01531337652732853</v>
       </c>
       <c r="B195">
-        <v>0.1858620400629406</v>
+        <v>0.1550450951418936</v>
       </c>
       <c r="C195">
         <v>1</v>
@@ -2533,10 +2533,10 @@
     </row>
     <row r="196" spans="1:3">
       <c r="A196">
-        <v>-0.1128202539316707</v>
+        <v>-0.1437527239044676</v>
       </c>
       <c r="B196">
-        <v>0.4457494887049651</v>
+        <v>0.442613971214782</v>
       </c>
       <c r="C196">
         <v>1</v>
@@ -2544,10 +2544,10 @@
     </row>
     <row r="197" spans="1:3">
       <c r="A197">
-        <v>-0.3733423305996922</v>
+        <v>-0.381310930885581</v>
       </c>
       <c r="B197">
-        <v>0.01439305269665348</v>
+        <v>-0.0148855172963262</v>
       </c>
       <c r="C197">
         <v>1</v>
@@ -2555,10 +2555,10 @@
     </row>
     <row r="198" spans="1:3">
       <c r="A198">
-        <v>-0.3971927686251533</v>
+        <v>-0.4061349020925686</v>
       </c>
       <c r="B198">
-        <v>-0.04693621252496791</v>
+        <v>-0.07481183932147788</v>
       </c>
       <c r="C198">
         <v>1</v>
@@ -2566,10 +2566,10 @@
     </row>
     <row r="199" spans="1:3">
       <c r="A199">
-        <v>-0.4417863770183662</v>
+        <v>-0.4582296807649885</v>
       </c>
       <c r="B199">
-        <v>0.2931423859224052</v>
+        <v>0.2868024752840524</v>
       </c>
       <c r="C199">
         <v>1</v>
@@ -2577,10 +2577,10 @@
     </row>
     <row r="200" spans="1:3">
       <c r="A200">
-        <v>-0.6678877817115584</v>
+        <v>-0.6180132039038554</v>
       </c>
       <c r="B200">
-        <v>-0.6312651386243011</v>
+        <v>-0.6452368359426225</v>
       </c>
       <c r="C200">
         <v>1</v>
@@ -2588,10 +2588,10 @@
     </row>
     <row r="201" spans="1:3">
       <c r="A201">
-        <v>-0.5116349720025382</v>
+        <v>-0.4544342529370739</v>
       </c>
       <c r="B201">
-        <v>-0.6823059753287178</v>
+        <v>-0.6803098431583323</v>
       </c>
       <c r="C201">
         <v>1</v>
@@ -2599,10 +2599,10 @@
     </row>
     <row r="202" spans="1:3">
       <c r="A202">
-        <v>-0.7340863900497698</v>
+        <v>-0.6967298088634069</v>
       </c>
       <c r="B202">
-        <v>-0.2244561674021507</v>
+        <v>-0.2256252917000872</v>
       </c>
       <c r="C202">
         <v>1</v>
@@ -2610,10 +2610,10 @@
     </row>
     <row r="203" spans="1:3">
       <c r="A203">
-        <v>1.251529032093554</v>
+        <v>1.260371392729269</v>
       </c>
       <c r="B203">
-        <v>0.07352861089843393</v>
+        <v>0.1614574003733772</v>
       </c>
       <c r="C203">
         <v>1</v>
@@ -2621,10 +2621,10 @@
     </row>
     <row r="204" spans="1:3">
       <c r="A204">
-        <v>1.204945753408002</v>
+        <v>1.222589434337062</v>
       </c>
       <c r="B204">
-        <v>0.05147410294382863</v>
+        <v>0.1521304936543308</v>
       </c>
       <c r="C204">
         <v>1</v>
@@ -2632,10 +2632,10 @@
     </row>
     <row r="205" spans="1:3">
       <c r="A205">
-        <v>1.217777527124085</v>
+        <v>1.227801691200437</v>
       </c>
       <c r="B205">
-        <v>0.1942199311339493</v>
+        <v>0.2852991796708506</v>
       </c>
       <c r="C205">
         <v>1</v>
@@ -2643,10 +2643,10 @@
     </row>
     <row r="206" spans="1:3">
       <c r="A206">
-        <v>-0.2272244903558424</v>
+        <v>-0.1956474427121755</v>
       </c>
       <c r="B206">
-        <v>-0.3916070059590549</v>
+        <v>-0.4056852729428785</v>
       </c>
       <c r="C206">
         <v>1</v>
@@ -2654,10 +2654,10 @@
     </row>
     <row r="207" spans="1:3">
       <c r="A207">
-        <v>-0.1366490226455163</v>
+        <v>-0.1132255623270335</v>
       </c>
       <c r="B207">
-        <v>-0.3196219176544566</v>
+        <v>-0.3337654505870497</v>
       </c>
       <c r="C207">
         <v>1</v>
@@ -2665,10 +2665,10 @@
     </row>
     <row r="208" spans="1:3">
       <c r="A208">
-        <v>-0.07947633871377849</v>
+        <v>-0.05973518523462122</v>
       </c>
       <c r="B208">
-        <v>-0.1247977943784928</v>
+        <v>-0.112476909891808</v>
       </c>
       <c r="C208">
         <v>1</v>
@@ -2676,10 +2676,10 @@
     </row>
     <row r="209" spans="1:3">
       <c r="A209">
-        <v>0.3045916388384635</v>
+        <v>0.3245303589249475</v>
       </c>
       <c r="B209">
-        <v>-0.4254982909080287</v>
+        <v>-0.4156895796527756</v>
       </c>
       <c r="C209">
         <v>1</v>
@@ -2687,10 +2687,10 @@
     </row>
     <row r="210" spans="1:3">
       <c r="A210">
-        <v>0.1953278178190705</v>
+        <v>0.2128669640189233</v>
       </c>
       <c r="B210">
-        <v>-0.5691593959404531</v>
+        <v>-0.5802146990801592</v>
       </c>
       <c r="C210">
         <v>1</v>
@@ -2698,10 +2698,10 @@
     </row>
     <row r="211" spans="1:3">
       <c r="A211">
-        <v>-0.03781343191952545</v>
+        <v>-0.03906255520756519</v>
       </c>
       <c r="B211">
-        <v>0.1619081092703924</v>
+        <v>0.1841076417790007</v>
       </c>
       <c r="C211">
         <v>1</v>
@@ -2709,10 +2709,10 @@
     </row>
     <row r="212" spans="1:3">
       <c r="A212">
-        <v>-0.1983100965491813</v>
+        <v>-0.1711968188255273</v>
       </c>
       <c r="B212">
-        <v>-0.4894143948731114</v>
+        <v>-0.5111626035182181</v>
       </c>
       <c r="C212">
         <v>1</v>
@@ -2720,10 +2720,10 @@
     </row>
     <row r="213" spans="1:3">
       <c r="A213">
-        <v>-0.1669488653617331</v>
+        <v>-0.1456066279353263</v>
       </c>
       <c r="B213">
-        <v>-0.5377932278241876</v>
+        <v>-0.5592406389604909</v>
       </c>
       <c r="C213">
         <v>1</v>
@@ -2731,10 +2731,10 @@
     </row>
     <row r="214" spans="1:3">
       <c r="A214">
-        <v>-0.2306036611381117</v>
+        <v>-0.2025541023964235</v>
       </c>
       <c r="B214">
-        <v>-0.1175203673194408</v>
+        <v>-0.09147365667372739</v>
       </c>
       <c r="C214">
         <v>1</v>
@@ -2742,10 +2742,10 @@
     </row>
     <row r="215" spans="1:3">
       <c r="A215">
-        <v>0.4487114112906388</v>
+        <v>0.4769461373395542</v>
       </c>
       <c r="B215">
-        <v>-0.1404166915314493</v>
+        <v>-0.1282746359867823</v>
       </c>
       <c r="C215">
         <v>1</v>
@@ -2753,10 +2753,10 @@
     </row>
     <row r="216" spans="1:3">
       <c r="A216">
-        <v>0.4304267186704991</v>
+        <v>0.4625672854568406</v>
       </c>
       <c r="B216">
-        <v>-0.1898564768255473</v>
+        <v>-0.1669986815024699</v>
       </c>
       <c r="C216">
         <v>1</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="217" spans="1:3">
       <c r="A217">
-        <v>0.3475514191285979</v>
+        <v>0.3754995555014879</v>
       </c>
       <c r="B217">
-        <v>0.07996893123915048</v>
+        <v>0.101158885833555</v>
       </c>
       <c r="C217">
         <v>1</v>
@@ -2775,10 +2775,10 @@
     </row>
     <row r="218" spans="1:3">
       <c r="A218">
-        <v>-0.02597398425904175</v>
+        <v>0.06811101154223356</v>
       </c>
       <c r="B218">
-        <v>-0.4940839543190471</v>
+        <v>0.08924918111461881</v>
       </c>
       <c r="C218">
         <v>1</v>
@@ -2786,10 +2786,10 @@
     </row>
     <row r="219" spans="1:3">
       <c r="A219">
-        <v>-0.09152439709327205</v>
+        <v>-0.06288798343482579</v>
       </c>
       <c r="B219">
-        <v>-0.2489245694940337</v>
+        <v>-0.02485324215486839</v>
       </c>
       <c r="C219">
         <v>1</v>
@@ -2797,10 +2797,10 @@
     </row>
     <row r="220" spans="1:3">
       <c r="A220">
-        <v>0.03229131386113496</v>
+        <v>-0.1859542142122843</v>
       </c>
       <c r="B220">
-        <v>-0.1471000618177778</v>
+        <v>0.2849129069904552</v>
       </c>
       <c r="C220">
         <v>1</v>
@@ -2808,10 +2808,10 @@
     </row>
     <row r="221" spans="1:3">
       <c r="A221">
-        <v>-0.2128434867766828</v>
+        <v>-0.2502939387898703</v>
       </c>
       <c r="B221">
-        <v>1.121446241499378</v>
+        <v>1.122880691877773</v>
       </c>
       <c r="C221">
         <v>1</v>
@@ -2819,10 +2819,10 @@
     </row>
     <row r="222" spans="1:3">
       <c r="A222">
-        <v>-0.1855452739931091</v>
+        <v>-0.2077455080434699</v>
       </c>
       <c r="B222">
-        <v>0.8450275175908297</v>
+        <v>0.8596509675069218</v>
       </c>
       <c r="C222">
         <v>1</v>
@@ -2830,10 +2830,10 @@
     </row>
     <row r="223" spans="1:3">
       <c r="A223">
-        <v>-0.2467717230730428</v>
+        <v>-0.2912822331512034</v>
       </c>
       <c r="B223">
-        <v>1.38305110827445</v>
+        <v>1.380188312235247</v>
       </c>
       <c r="C223">
         <v>1</v>
@@ -2841,10 +2841,10 @@
     </row>
     <row r="224" spans="1:3">
       <c r="A224">
-        <v>-1.161366489138713</v>
+        <v>-1.13726379126366</v>
       </c>
       <c r="B224">
-        <v>0.003525039373194707</v>
+        <v>-0.01012772315687389</v>
       </c>
       <c r="C224">
         <v>1</v>
@@ -2852,10 +2852,10 @@
     </row>
     <row r="225" spans="1:3">
       <c r="A225">
-        <v>-1.095884940342948</v>
+        <v>-1.062322536150349</v>
       </c>
       <c r="B225">
-        <v>-0.003512191142145654</v>
+        <v>-0.0274947050818973</v>
       </c>
       <c r="C225">
         <v>1</v>
@@ -2863,10 +2863,10 @@
     </row>
     <row r="226" spans="1:3">
       <c r="A226">
-        <v>-1.138505111390219</v>
+        <v>-1.118659358391127</v>
       </c>
       <c r="B226">
-        <v>0.07077582038933428</v>
+        <v>0.05660837172319726</v>
       </c>
       <c r="C226">
         <v>1</v>
@@ -2874,10 +2874,10 @@
     </row>
     <row r="227" spans="1:3">
       <c r="A227">
-        <v>-0.1958976532489778</v>
+        <v>-0.1693115033400768</v>
       </c>
       <c r="B227">
-        <v>-0.6222630146532171</v>
+        <v>-0.6348185709264829</v>
       </c>
       <c r="C227">
         <v>1</v>
@@ -2885,10 +2885,10 @@
     </row>
     <row r="228" spans="1:3">
       <c r="A228">
-        <v>-0.06128970337603217</v>
+        <v>-0.0243709247361962</v>
       </c>
       <c r="B228">
-        <v>-0.7300967736119465</v>
+        <v>-0.7371874339702827</v>
       </c>
       <c r="C228">
         <v>1</v>
@@ -2896,10 +2896,10 @@
     </row>
     <row r="229" spans="1:3">
       <c r="A229">
-        <v>-0.1211334597625678</v>
+        <v>-0.09640162259007139</v>
       </c>
       <c r="B229">
-        <v>-0.2327775890830219</v>
+        <v>-0.1956831117628826</v>
       </c>
       <c r="C229">
         <v>1</v>
@@ -2907,10 +2907,10 @@
     </row>
     <row r="230" spans="1:3">
       <c r="A230">
-        <v>-0.033420289519071</v>
+        <v>0.09318630090729228</v>
       </c>
       <c r="B230">
-        <v>-0.3055942423837686</v>
+        <v>-0.4710820572181043</v>
       </c>
       <c r="C230">
         <v>1</v>
@@ -2918,10 +2918,10 @@
     </row>
     <row r="231" spans="1:3">
       <c r="A231">
-        <v>-0.1975826379062214</v>
+        <v>0.01576694059527042</v>
       </c>
       <c r="B231">
-        <v>-0.09255805036361232</v>
+        <v>-0.4384813666574545</v>
       </c>
       <c r="C231">
         <v>1</v>
@@ -2929,10 +2929,10 @@
     </row>
     <row r="232" spans="1:3">
       <c r="A232">
-        <v>0.05341507388684444</v>
+        <v>-0.05805390293130065</v>
       </c>
       <c r="B232">
-        <v>-0.01413348405677899</v>
+        <v>-0.1710537461464081</v>
       </c>
       <c r="C232">
         <v>1</v>
@@ -2940,10 +2940,10 @@
     </row>
     <row r="233" spans="1:3">
       <c r="A233">
-        <v>0.3832360783864495</v>
+        <v>0.4209280237295242</v>
       </c>
       <c r="B233">
-        <v>-0.3943513117965906</v>
+        <v>-0.3890793330478048</v>
       </c>
       <c r="C233">
         <v>1</v>
@@ -2951,10 +2951,10 @@
     </row>
     <row r="234" spans="1:3">
       <c r="A234">
-        <v>0.4376500282211196</v>
+        <v>0.4666616142729678</v>
       </c>
       <c r="B234">
-        <v>-0.2439954254981071</v>
+        <v>-0.2462688788290941</v>
       </c>
       <c r="C234">
         <v>1</v>
@@ -2962,10 +2962,10 @@
     </row>
     <row r="235" spans="1:3">
       <c r="A235">
-        <v>0.3987601638394906</v>
+        <v>0.4124285413627271</v>
       </c>
       <c r="B235">
-        <v>-0.2385371048224275</v>
+        <v>-0.2413450165504781</v>
       </c>
       <c r="C235">
         <v>1</v>
@@ -2973,10 +2973,10 @@
     </row>
     <row r="236" spans="1:3">
       <c r="A236">
-        <v>-0.1996835591050258</v>
+        <v>-0.1912567268698641</v>
       </c>
       <c r="B236">
-        <v>-0.5225253419839861</v>
+        <v>-0.5443873916997183</v>
       </c>
       <c r="C236">
         <v>1</v>
@@ -2984,10 +2984,10 @@
     </row>
     <row r="237" spans="1:3">
       <c r="A237">
-        <v>-0.2117325391162855</v>
+        <v>-0.2046301244124588</v>
       </c>
       <c r="B237">
-        <v>-0.4129749254031363</v>
+        <v>-0.4122067669981401</v>
       </c>
       <c r="C237">
         <v>1</v>
@@ -2995,10 +2995,10 @@
     </row>
     <row r="238" spans="1:3">
       <c r="A238">
-        <v>-0.224679576229966</v>
+        <v>-0.2314820878109808</v>
       </c>
       <c r="B238">
-        <v>-0.2481433512644835</v>
+        <v>-0.2546246130503651</v>
       </c>
       <c r="C238">
         <v>1</v>
@@ -3006,10 +3006,10 @@
     </row>
     <row r="239" spans="1:3">
       <c r="A239">
-        <v>-0.756329989370874</v>
+        <v>-0.7706504808581521</v>
       </c>
       <c r="B239">
-        <v>0.2054063071639987</v>
+        <v>0.1435928144626816</v>
       </c>
       <c r="C239">
         <v>1</v>
@@ -3017,10 +3017,10 @@
     </row>
     <row r="240" spans="1:3">
       <c r="A240">
-        <v>-0.9132235567580935</v>
+        <v>-0.9313106640658235</v>
       </c>
       <c r="B240">
-        <v>0.1719709656952488</v>
+        <v>0.1222478164144935</v>
       </c>
       <c r="C240">
         <v>1</v>
@@ -3028,10 +3028,10 @@
     </row>
     <row r="241" spans="1:3">
       <c r="A241">
-        <v>-0.8993361983260162</v>
+        <v>-0.9299326982519992</v>
       </c>
       <c r="B241">
-        <v>0.5690369972716317</v>
+        <v>0.5317045679247371</v>
       </c>
       <c r="C241">
         <v>1</v>
@@ -3039,10 +3039,10 @@
     </row>
     <row r="242" spans="1:3">
       <c r="A242">
-        <v>0.6339012728962994</v>
+        <v>0.5953354207842068</v>
       </c>
       <c r="B242">
-        <v>1.611178238764871</v>
+        <v>1.598264336743031</v>
       </c>
       <c r="C242">
         <v>1</v>
@@ -3050,10 +3050,10 @@
     </row>
     <row r="243" spans="1:3">
       <c r="A243">
-        <v>0.836743571488071</v>
+        <v>0.7706669878436063</v>
       </c>
       <c r="B243">
-        <v>1.640507115396955</v>
+        <v>1.612031474132539</v>
       </c>
       <c r="C243">
         <v>1</v>
@@ -3061,10 +3061,10 @@
     </row>
     <row r="244" spans="1:3">
       <c r="A244">
-        <v>0.623126380066652</v>
+        <v>0.586392282065579</v>
       </c>
       <c r="B244">
-        <v>1.773073057733524</v>
+        <v>1.765901123681204</v>
       </c>
       <c r="C244">
         <v>1</v>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="245" spans="1:3">
       <c r="A245">
-        <v>0.806521029184785</v>
+        <v>0.8393547028599421</v>
       </c>
       <c r="B245">
-        <v>-0.7254196583278132</v>
+        <v>-0.6861254465160306</v>
       </c>
       <c r="C245">
         <v>1</v>
@@ -3083,10 +3083,10 @@
     </row>
     <row r="246" spans="1:3">
       <c r="A246">
-        <v>0.7371215177010356</v>
+        <v>0.7690461735987256</v>
       </c>
       <c r="B246">
-        <v>-0.7346215208723857</v>
+        <v>-0.6966774502934819</v>
       </c>
       <c r="C246">
         <v>1</v>
@@ -3094,10 +3094,10 @@
     </row>
     <row r="247" spans="1:3">
       <c r="A247">
-        <v>0.4746867719036172</v>
+        <v>0.4954405149257536</v>
       </c>
       <c r="B247">
-        <v>-0.2367667590886686</v>
+        <v>-0.210289063553773</v>
       </c>
       <c r="C247">
         <v>1</v>
@@ -3105,10 +3105,10 @@
     </row>
     <row r="248" spans="1:3">
       <c r="A248">
-        <v>-0.4979890623394749</v>
+        <v>-0.5262246386535416</v>
       </c>
       <c r="B248">
-        <v>0.09254198112557903</v>
+        <v>0.04577679586732662</v>
       </c>
       <c r="C248">
         <v>1</v>
@@ -3116,10 +3116,10 @@
     </row>
     <row r="249" spans="1:3">
       <c r="A249">
-        <v>-0.5400074232890607</v>
+        <v>-0.5528838862987221</v>
       </c>
       <c r="B249">
-        <v>-0.01821737227756507</v>
+        <v>-0.05462549781152527</v>
       </c>
       <c r="C249">
         <v>1</v>
@@ -3127,10 +3127,10 @@
     </row>
     <row r="250" spans="1:3">
       <c r="A250">
-        <v>-0.2733927735675588</v>
+        <v>-0.2879975631813552</v>
       </c>
       <c r="B250">
-        <v>0.3289179358340277</v>
+        <v>0.3201444657960754</v>
       </c>
       <c r="C250">
         <v>1</v>
@@ -3138,10 +3138,10 @@
     </row>
     <row r="251" spans="1:3">
       <c r="A251">
-        <v>-0.4897789830573639</v>
+        <v>-0.4840273378114465</v>
       </c>
       <c r="B251">
-        <v>-0.4923046896063033</v>
+        <v>-0.5693875087801659</v>
       </c>
       <c r="C251">
         <v>1</v>
@@ -3149,10 +3149,10 @@
     </row>
     <row r="252" spans="1:3">
       <c r="A252">
-        <v>-0.5896841349563307</v>
+        <v>-0.5934715595064248</v>
       </c>
       <c r="B252">
-        <v>-0.4058570534469297</v>
+        <v>-0.4634259056596115</v>
       </c>
       <c r="C252">
         <v>1</v>
@@ -3160,10 +3160,10 @@
     </row>
     <row r="253" spans="1:3">
       <c r="A253">
-        <v>-0.4120748214263197</v>
+        <v>-0.3993493891395065</v>
       </c>
       <c r="B253">
-        <v>-0.3677182748280898</v>
+        <v>-0.4214061473661987</v>
       </c>
       <c r="C253">
         <v>1</v>
@@ -3171,10 +3171,10 @@
     </row>
     <row r="254" spans="1:3">
       <c r="A254">
-        <v>-0.5982048734407135</v>
+        <v>-0.5529556206360373</v>
       </c>
       <c r="B254">
-        <v>-0.6083772955921728</v>
+        <v>-0.5968699028012926</v>
       </c>
       <c r="C254">
         <v>1</v>
@@ -3182,10 +3182,10 @@
     </row>
     <row r="255" spans="1:3">
       <c r="A255">
-        <v>-0.5706949387137237</v>
+        <v>-0.4447329649948069</v>
       </c>
       <c r="B255">
-        <v>-0.5113209494558737</v>
+        <v>-0.6867406202390303</v>
       </c>
       <c r="C255">
         <v>1</v>
@@ -3193,10 +3193,10 @@
     </row>
     <row r="256" spans="1:3">
       <c r="A256">
-        <v>-0.5004917412305326</v>
+        <v>-0.4699475203038037</v>
       </c>
       <c r="B256">
-        <v>-0.2118202874070386</v>
+        <v>-0.1780763633889038</v>
       </c>
       <c r="C256">
         <v>1</v>
@@ -3204,10 +3204,10 @@
     </row>
     <row r="257" spans="1:3">
       <c r="A257">
-        <v>-0.1198956187260157</v>
+        <v>-0.1255503907686747</v>
       </c>
       <c r="B257">
-        <v>0.2372851344411416</v>
+        <v>0.2333501652807524</v>
       </c>
       <c r="C257">
         <v>1</v>
@@ -3215,10 +3215,10 @@
     </row>
     <row r="258" spans="1:3">
       <c r="A258">
-        <v>0.1395599340175815</v>
+        <v>0.1537743531537295</v>
       </c>
       <c r="B258">
-        <v>-0.2383558022232584</v>
+        <v>-0.2348709399649784</v>
       </c>
       <c r="C258">
         <v>1</v>
@@ -3226,10 +3226,10 @@
     </row>
     <row r="259" spans="1:3">
       <c r="A259">
-        <v>-0.2071793361939581</v>
+        <v>-0.2082787156153628</v>
       </c>
       <c r="B259">
-        <v>0.4270089320977306</v>
+        <v>0.4208035170473277</v>
       </c>
       <c r="C259">
         <v>1</v>
@@ -3237,10 +3237,10 @@
     </row>
     <row r="260" spans="1:3">
       <c r="A260">
-        <v>-0.08952787705140701</v>
+        <v>-0.09710597007799189</v>
       </c>
       <c r="B260">
-        <v>-0.1297525066761493</v>
+        <v>-0.1559698744039974</v>
       </c>
       <c r="C260">
         <v>1</v>
@@ -3248,10 +3248,10 @@
     </row>
     <row r="261" spans="1:3">
       <c r="A261">
-        <v>0.1228959986739231</v>
+        <v>0.1313083158088282</v>
       </c>
       <c r="B261">
-        <v>-0.329990457996192</v>
+        <v>-0.3215046174758344</v>
       </c>
       <c r="C261">
         <v>1</v>
@@ -3259,10 +3259,10 @@
     </row>
     <row r="262" spans="1:3">
       <c r="A262">
-        <v>-0.3019363899632143</v>
+        <v>-0.3189238134115336</v>
       </c>
       <c r="B262">
-        <v>0.3550081769654164</v>
+        <v>0.3562831645300358</v>
       </c>
       <c r="C262">
         <v>1</v>
@@ -3270,10 +3270,10 @@
     </row>
     <row r="263" spans="1:3">
       <c r="A263">
-        <v>0.3606106231604383</v>
+        <v>0.3582070944716334</v>
       </c>
       <c r="B263">
-        <v>-0.1851718430851285</v>
+        <v>-0.2174155987130714</v>
       </c>
       <c r="C263">
         <v>1</v>
@@ -3281,10 +3281,10 @@
     </row>
     <row r="264" spans="1:3">
       <c r="A264">
-        <v>0.3853293832543428</v>
+        <v>0.3835321373540912</v>
       </c>
       <c r="B264">
-        <v>0.09540425872463694</v>
+        <v>0.08061701098352679</v>
       </c>
       <c r="C264">
         <v>1</v>
@@ -3292,10 +3292,10 @@
     </row>
     <row r="265" spans="1:3">
       <c r="A265">
-        <v>0.2730284932712504</v>
+        <v>0.2405300837389333</v>
       </c>
       <c r="B265">
-        <v>0.311392045826401</v>
+        <v>0.2634949874958882</v>
       </c>
       <c r="C265">
         <v>1</v>
@@ -3303,10 +3303,10 @@
     </row>
     <row r="266" spans="1:3">
       <c r="A266">
-        <v>0.2790175792964276</v>
+        <v>0.2604924627044717</v>
       </c>
       <c r="B266">
-        <v>-0.05540159789554003</v>
+        <v>-0.02201699705440015</v>
       </c>
       <c r="C266">
         <v>1</v>
@@ -3314,10 +3314,10 @@
     </row>
     <row r="267" spans="1:3">
       <c r="A267">
-        <v>0.2065869702592756</v>
+        <v>0.1871472377148622</v>
       </c>
       <c r="B267">
-        <v>-0.128756855864806</v>
+        <v>-0.09707465634212491</v>
       </c>
       <c r="C267">
         <v>1</v>
@@ -3325,10 +3325,10 @@
     </row>
     <row r="268" spans="1:3">
       <c r="A268">
-        <v>0.08817278632601748</v>
+        <v>0.07274226367690921</v>
       </c>
       <c r="B268">
-        <v>0.2270992944222561</v>
+        <v>0.2513149569531702</v>
       </c>
       <c r="C268">
         <v>1</v>
@@ -3336,10 +3336,10 @@
     </row>
     <row r="269" spans="1:3">
       <c r="A269">
-        <v>-0.2158642390273589</v>
+        <v>-0.1984057446959379</v>
       </c>
       <c r="B269">
-        <v>-0.3428413068628674</v>
+        <v>-0.3549225929199393</v>
       </c>
       <c r="C269">
         <v>1</v>
@@ -3347,10 +3347,10 @@
     </row>
     <row r="270" spans="1:3">
       <c r="A270">
-        <v>-0.05004198382892003</v>
+        <v>-0.02947113930665008</v>
       </c>
       <c r="B270">
-        <v>-0.4488833695059056</v>
+        <v>-0.4356942526577872</v>
       </c>
       <c r="C270">
         <v>1</v>
@@ -3358,10 +3358,10 @@
     </row>
     <row r="271" spans="1:3">
       <c r="A271">
-        <v>-0.2722191072049222</v>
+        <v>-0.2648817284567132</v>
       </c>
       <c r="B271">
-        <v>0.02588561766591046</v>
+        <v>0.01798086372048908</v>
       </c>
       <c r="C271">
         <v>1</v>

</xml_diff>